<commit_message>
Leaderboard button image changed.
</commit_message>
<xml_diff>
--- a/План доработок.xlsx
+++ b/План доработок.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/v_triputin/AndroidStudioProjects/CradleOfTronesGDX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F297E3-21EA-684C-9D59-5B98860A1987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445F672B-70F8-4E43-9AC7-7407764364B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{342D1634-4B6E-1C49-B973-0F169133A098}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Если выделено, то нельзя отменить выделение</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>По завершению атаки, в случае победы, предлагать удвоить результат за просмотр видео.</t>
+  </si>
+  <si>
+    <t>Статус</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -150,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -173,6 +179,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F451F162-DA5E-CB4E-80A2-CA53019693C0}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,16 +508,20 @@
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="2" width="58.33203125" customWidth="1"/>
     <col min="3" max="3" width="59.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -516,8 +529,9 @@
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -527,8 +541,11 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -538,8 +555,9 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -547,8 +565,9 @@
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -556,8 +575,9 @@
         <v>3</v>
       </c>
       <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -565,6 +585,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2"/>
+      <c r="D7" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Target of attack view added.
</commit_message>
<xml_diff>
--- a/План доработок.xlsx
+++ b/План доработок.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/v_triputin/AndroidStudioProjects/CradleOfTronesGDX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445F672B-70F8-4E43-9AC7-7407764364B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA83651E-2782-924C-8FD5-AD518B094CFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{342D1634-4B6E-1C49-B973-0F169133A098}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Доработки" sheetId="1" r:id="rId1"/>
+    <sheet name="Разрешения экрана" sheetId="2" r:id="rId2"/>
+    <sheet name="Цели" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Если выделено, то нельзя отменить выделение</t>
   </si>
@@ -66,13 +68,103 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>xiaomi mi9</t>
+  </si>
+  <si>
+    <r>
+      <t>Экран: диагональ 6,39", разрешение 2340 х 1080 точки, 19.5:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, ppi 403.</t>
+    </r>
+  </si>
+  <si>
+    <t>huawei amn-lx9</t>
+  </si>
+  <si>
+    <t>Размер экрана‎: ‎5.71"    Разрешение экрана‎: ‎720x1520</t>
+  </si>
+  <si>
+    <t>Pixel</t>
+  </si>
+  <si>
+    <t>1920x1080</t>
+  </si>
+  <si>
+    <t>2880x1440</t>
+  </si>
+  <si>
+    <t>Pixel 2XL</t>
+  </si>
+  <si>
+    <t>Nexus S</t>
+  </si>
+  <si>
+    <t>4" ,  800x480</t>
+  </si>
+  <si>
+    <t>1280x768</t>
+  </si>
+  <si>
+    <t>Nexus 4</t>
+  </si>
+  <si>
+    <t>854x480</t>
+  </si>
+  <si>
+    <t>FWVGA</t>
+  </si>
+  <si>
+    <t>2560x1440</t>
+  </si>
+  <si>
+    <t>Nexus 6</t>
+  </si>
+  <si>
+    <t>Напоминание что надо обновить игру с переходом на гугл плэй с бонусом в виде золота.</t>
+  </si>
+  <si>
+    <t>Cделать после набора активной игровой базы.</t>
+  </si>
+  <si>
+    <t>Разрушить</t>
+  </si>
+  <si>
+    <t>Цель атаки</t>
+  </si>
+  <si>
+    <t>Продолжить</t>
+  </si>
+  <si>
+    <t>После нажатия на продолжить раскрывается поле SetVisible.</t>
+  </si>
+  <si>
+    <t>Х</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,8 +180,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,8 +214,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -152,11 +282,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -177,11 +387,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,15 +761,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F451F162-DA5E-CB4E-80A2-CA53019693C0}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
     <col min="2" max="2" width="58.33203125" customWidth="1"/>
     <col min="3" max="3" width="59.6640625" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" customWidth="1"/>
@@ -529,7 +793,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="9"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -541,11 +805,11 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -555,7 +819,9 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -565,27 +831,39 @@
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="9"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="9"/>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -593,4 +871,177 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE8DE78-552C-3E4E-B01F-23B0FDA3A317}">
+  <dimension ref="A2:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="114.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="25" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="25" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="25" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="25" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="25" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="25" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="25" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C686F8-D3E2-6247-88A3-8B1FE8918C8C}">
+  <dimension ref="A3:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="8" max="8" width="4.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="G7" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="25"/>
+      <c r="I7" s="26"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B9" s="17"/>
+      <c r="C9" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="G9" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="29"/>
+    </row>
+    <row r="10" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="B10" s="14"/>
+      <c r="C10" s="20">
+        <v>3</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="G10" s="30">
+        <v>3</v>
+      </c>
+      <c r="H10" s="15"/>
+      <c r="I10" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="23"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G9:I9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Dialog about target of attack view added.
</commit_message>
<xml_diff>
--- a/План доработок.xlsx
+++ b/План доработок.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/v_triputin/AndroidStudioProjects/CradleOfTronesGDX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA83651E-2782-924C-8FD5-AD518B094CFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08133096-210E-7647-B131-EEB95AB1D2A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{342D1634-4B6E-1C49-B973-0F169133A098}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="1" xr2:uid="{342D1634-4B6E-1C49-B973-0F169133A098}"/>
   </bookViews>
   <sheets>
     <sheet name="Доработки" sheetId="1" r:id="rId1"/>
-    <sheet name="Разрешения экрана" sheetId="2" r:id="rId2"/>
-    <sheet name="Цели" sheetId="3" r:id="rId3"/>
+    <sheet name="Аналитика" sheetId="4" r:id="rId2"/>
+    <sheet name="Разрешения экрана" sheetId="2" r:id="rId3"/>
+    <sheet name="Цели" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Если выделено, то нельзя отменить выделение</t>
   </si>
@@ -159,12 +160,48 @@
   <si>
     <t>Х</t>
   </si>
+  <si>
+    <t>Показывать что используй булаву</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Собери ресурсы над всеми оранжевыми ячейками для победы! </t>
+  </si>
+  <si>
+    <t>Собрать ресурсы можно соединив 3 и более в ряд одинаковых ресурса.</t>
+  </si>
+  <si>
+    <t>Серебряная монета может быть собрана с любым ресурсом.</t>
+  </si>
+  <si>
+    <t>После согласия на рестарт, сразу перенаправлять на экран с кнопкой старт!</t>
+  </si>
+  <si>
+    <t>Добавить события отдельные, что пройден первый уровнеь, второй. Третий , четверый. Для анализа в аналитике.</t>
+  </si>
+  <si>
+    <t>На втором уровне подсказка - можно купить бомбу в магазине</t>
+  </si>
+  <si>
+    <t>На третьем - купить гранату</t>
+  </si>
+  <si>
+    <t>Событие что деньги собраны с замка</t>
+  </si>
+  <si>
+    <t>Удержание пользователей</t>
+  </si>
+  <si>
+    <t>1день - 10,1%, 2й-4,6%, 3й-3%, 4й-2%</t>
+  </si>
+  <si>
+    <t>последние 42 дня, до апр. 30 ( 19.03-30.04)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -199,6 +236,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -366,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -447,6 +491,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F451F162-DA5E-CB4E-80A2-CA53019693C0}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -795,85 +844,177 @@
       <c r="C2" s="2"/>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="5" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B13" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="C13" s="5"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B15" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="8"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE426184-AF6D-7748-89CB-210B4FA924E8}">
+  <dimension ref="B2:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE8DE78-552C-3E4E-B01F-23B0FDA3A317}">
   <dimension ref="A2:B9"/>
   <sheetViews>
@@ -956,23 +1097,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C686F8-D3E2-6247-88A3-8B1FE8918C8C}">
-  <dimension ref="A3:I15"/>
+  <dimension ref="A3:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.1640625" customWidth="1"/>
     <col min="8" max="8" width="4.1640625" customWidth="1"/>
+    <col min="12" max="12" width="40" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="24" t="s">
         <v>30</v>
       </c>
@@ -983,16 +1126,22 @@
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="26"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L7" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="26"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
       <c r="G8" s="14"/>
       <c r="H8" s="15"/>
       <c r="I8" s="16"/>
-    </row>
-    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="L8" s="14"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.2">
       <c r="B9" s="17"/>
       <c r="C9" s="18" t="s">
         <v>29</v>
@@ -1003,8 +1152,12 @@
       </c>
       <c r="H9" s="27"/>
       <c r="I9" s="29"/>
-    </row>
-    <row r="10" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="L9" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B10" s="14"/>
       <c r="C10" s="20">
         <v>3</v>
@@ -1017,30 +1170,49 @@
       <c r="I10" s="31">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L10" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="16"/>
+    </row>
+    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B11" s="21"/>
       <c r="C11" s="22"/>
       <c r="D11" s="23"/>
       <c r="G11" s="21"/>
       <c r="H11" s="22"/>
       <c r="I11" s="23"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L11" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="16"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L12" s="14"/>
+      <c r="M12" s="16"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L13" s="14"/>
+      <c r="M13" s="16"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L14" s="21"/>
+      <c r="M14" s="23"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G9:I9"/>
+    <mergeCell ref="L7:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Use weapon arrow added.
</commit_message>
<xml_diff>
--- a/План доработок.xlsx
+++ b/План доработок.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/v_triputin/AndroidStudioProjects/CradleOfTronesGDX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08133096-210E-7647-B131-EEB95AB1D2A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1530750D-77F5-7045-931F-C1A185D9E23E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="1" xr2:uid="{342D1634-4B6E-1C49-B973-0F169133A098}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Если выделено, то нельзя отменить выделение</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t xml:space="preserve">Над часами сделать блок. </t>
-  </si>
-  <si>
-    <t>Cделать диалоговое окно перед началом атаки ( Цель ), но должно сначала сфорироваться поле, потом появляется окно.</t>
   </si>
   <si>
     <t>По завершению атаки, в случае победы, предлагать удвоить результат за просмотр видео.</t>
@@ -176,9 +173,6 @@
     <t>После согласия на рестарт, сразу перенаправлять на экран с кнопкой старт!</t>
   </si>
   <si>
-    <t>Добавить события отдельные, что пройден первый уровнеь, второй. Третий , четверый. Для анализа в аналитике.</t>
-  </si>
-  <si>
     <t>На втором уровне подсказка - можно купить бомбу в магазине</t>
   </si>
   <si>
@@ -195,13 +189,50 @@
   </si>
   <si>
     <t>последние 42 дня, до апр. 30 ( 19.03-30.04)</t>
+  </si>
+  <si>
+    <t>Добавить события отдельные, что пройден первый уровень, второй. Третий , четверый. Для анализа в аналитике.</t>
+  </si>
+  <si>
+    <t>Cделать диалоговое окно перед началом атаки ( Цель ), но должно сначала сформироваться поле, потом появляется окно.</t>
+  </si>
+  <si>
+    <t>% пользователей выигравших одну атаку (level up)</t>
+  </si>
+  <si>
+    <t>март 2020</t>
+  </si>
+  <si>
+    <t>апрель 2020</t>
+  </si>
+  <si>
+    <t>При нажатии на замок в месте бомбы  - надпись Закрыто. Возможность появится на уровне X.</t>
+  </si>
+  <si>
+    <t>Надпись исчезает после первого сбора (флжок должен сохраняться)</t>
+  </si>
+  <si>
+    <t>Надпись исчезает после первого использования (флжок должен сохраняться)</t>
+  </si>
+  <si>
+    <t>% утраченных к новым пользователей в первый день</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -243,6 +274,12 @@
       <color theme="1"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -407,16 +444,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -434,17 +472,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -461,7 +496,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -485,20 +520,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -810,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F451F162-DA5E-CB4E-80A2-CA53019693C0}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -831,49 +875,57 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="1">
+        <v>5</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="8"/>
@@ -881,7 +933,7 @@
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="8"/>
@@ -889,90 +941,94 @@
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="4"/>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>3</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>4</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>5</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="8"/>
+      <c r="D12" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>6</v>
-      </c>
+      <c r="A14" s="1"/>
       <c r="B14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="C15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="5"/>
       <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>7</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -980,36 +1036,89 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE426184-AF6D-7748-89CB-210B4FA924E8}">
-  <dimension ref="B2:G7"/>
+  <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="45.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="34" t="s">
-        <v>43</v>
+      <c r="B2" s="33" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="36">
+        <f>128/1038</f>
+        <v>0.1233140655105973</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="36">
+        <f>145/524</f>
+        <v>0.27671755725190839</v>
+      </c>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C12" s="32">
+        <v>43948</v>
+      </c>
+      <c r="D12" s="35">
+        <f>94/243</f>
+        <v>0.38683127572016462</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C13" s="32">
+        <v>43949</v>
+      </c>
+      <c r="D13" s="35">
+        <f>132/181</f>
+        <v>0.72928176795580113</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C14" s="32">
+        <v>43950</v>
+      </c>
+      <c r="D14" s="34">
+        <f>67/5</f>
+        <v>13.4</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1030,66 +1139,66 @@
   <sheetData>
     <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="25" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="25" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="25" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="25" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="25" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="25" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="25" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1113,98 +1222,98 @@
     <col min="13" max="13" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="G7" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26"/>
-      <c r="L7" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="M7" s="26"/>
+      <c r="B7" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="G7" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="24"/>
+      <c r="I7" s="25"/>
+      <c r="L7" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="25"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="16"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="15"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.2">
-      <c r="B9" s="17"/>
-      <c r="C9" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="19"/>
-      <c r="G9" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="29"/>
-      <c r="L9" s="32" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="G9" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="26"/>
+      <c r="I9" s="28"/>
+      <c r="L9" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="B10" s="13"/>
+      <c r="C10" s="19">
+        <v>3</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="G10" s="29">
+        <v>3</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="30">
+        <v>2</v>
+      </c>
+      <c r="L10" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="M9" s="16"/>
-    </row>
-    <row r="10" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="B10" s="14"/>
-      <c r="C10" s="20">
-        <v>3</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="G10" s="30">
-        <v>3</v>
-      </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="31">
-        <v>2</v>
-      </c>
-      <c r="L10" s="17" t="s">
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="22"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="22"/>
+      <c r="L11" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="M10" s="16"/>
-    </row>
-    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
-      <c r="L11" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="M11" s="16"/>
+      <c r="M11" s="15"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L12" s="14"/>
-      <c r="M12" s="16"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="15"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="16"/>
+        <v>30</v>
+      </c>
+      <c r="L13" s="13"/>
+      <c r="M13" s="15"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L14" s="21"/>
-      <c r="M14" s="23"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="22"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use weapon arrow improved.
</commit_message>
<xml_diff>
--- a/План доработок.xlsx
+++ b/План доработок.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/v_triputin/AndroidStudioProjects/CradleOfTronesGDX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1530750D-77F5-7045-931F-C1A185D9E23E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C805585-BEF2-FA49-BE48-55AAFD4B3AC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="1" xr2:uid="{342D1634-4B6E-1C49-B973-0F169133A098}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{342D1634-4B6E-1C49-B973-0F169133A098}"/>
   </bookViews>
   <sheets>
     <sheet name="Доработки" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Если выделено, то нельзя отменить выделение</t>
   </si>
@@ -209,13 +209,13 @@
     <t>При нажатии на замок в месте бомбы  - надпись Закрыто. Возможность появится на уровне X.</t>
   </si>
   <si>
-    <t>Надпись исчезает после первого сбора (флжок должен сохраняться)</t>
-  </si>
-  <si>
-    <t>Надпись исчезает после первого использования (флжок должен сохраняться)</t>
-  </si>
-  <si>
     <t>% утраченных к новым пользователей в первый день</t>
+  </si>
+  <si>
+    <t>Надпись исчезает после первого использования (флажок должен сохраняться)</t>
+  </si>
+  <si>
+    <t>Надпись исчезает после первого сбора (флажок должен сохраняться)</t>
   </si>
 </sst>
 </file>
@@ -856,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F451F162-DA5E-CB4E-80A2-CA53019693C0}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,7 +888,9 @@
       <c r="C2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -898,7 +900,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D3" s="8"/>
     </row>
@@ -1038,7 +1040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE426184-AF6D-7748-89CB-210B4FA924E8}">
   <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1087,7 +1089,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
@@ -1211,7 +1213,7 @@
   <dimension ref="A3:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Types of attack added. Steps and time.
</commit_message>
<xml_diff>
--- a/План доработок.xlsx
+++ b/План доработок.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/v_triputin/AndroidStudioProjects/CradleOfTronesGDX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C805585-BEF2-FA49-BE48-55AAFD4B3AC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71C5E66-0964-EF4D-807A-07CC69E66209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{342D1634-4B6E-1C49-B973-0F169133A098}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Разрешения экрана" sheetId="2" r:id="rId3"/>
     <sheet name="Цели" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
   <si>
     <t>Если выделено, то нельзя отменить выделение</t>
   </si>
@@ -217,13 +217,71 @@
   <si>
     <t>Надпись исчезает после первого сбора (флажок должен сохраняться)</t>
   </si>
+  <si>
+    <t>Tip of the day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Окно при старте ( описание элемента игры) С подсчетом какие уже показаны. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Если нехватает ресурсов для атаки показать другое окно , в котором надпись не хватает таких-то ресурсов для атаки. Можно заработать ресурсы на арене или обменять в магазине.  </t>
+  </si>
+  <si>
+    <t>Добавить награды за 5 подряд, 6 подряд</t>
+  </si>
+  <si>
+    <t>Горизонтальная бомба - взрыв по горизонтали, верт бомба взрыв по вертикали (способ применения - собрать бомбу(т.е. Заряженный элемент в ряд не менее 3-х!) Бомба которая взрывает все такого же типа как собранные с ней.</t>
+  </si>
+  <si>
+    <t>Не хватает мотивации на следующую атаку. Во временах года, периодически бонусы и прочее игрок может видеть что его чтото ждет новое далее.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Для атаки не хватает:    
+Можно заработать ресурсы на арене или обменять в магазине.  </t>
+  </si>
+  <si>
+    <t>Это уже ваш замок при нажатии на свой замок</t>
+  </si>
+  <si>
+    <t>Сообщение есть но оно отключено т.к. мешает сбору золота?</t>
+  </si>
+  <si>
+    <t>При проигрыше атаки, предложить выбор или докупить 10 сек за 100 монет или в магазин за покупкой монет или 20 сек за просмотр ролика</t>
+  </si>
+  <si>
+    <t>1) Добавить главный замок на карту.
+2) Можно атаковать после захвата остальных. 
+3) В замке герой который играет против ( босс ). 
+4) С каждым уровнем атаки растет уровень сопротивления босса, т.е. Он выбирает все лучший и лучший вариант ответа. Игра пошаговая босс-игрок, цель набрать столько-то очков. Кто первый набрал тот и выиграл.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - X
+2) - X
+3) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DialogBox_NotEnoughSteps - доделать!!!</t>
+  </si>
+  <si>
+    <t>Если не хватило ходов, то предложить доп 5 ходов (доп 10 сек)  за просмотр рекламы или докупить 5 ходов (10сек) за ?</t>
+  </si>
+  <si>
+    <t>Или цель - убить босса, чем больше собрал ресов тем сильнее удар. Или удар только за кристаллы!?
+Герой игрока - его уровень жизни уменьшается после ударов босса. Если уровень жизни упал до 0 то проигрыш, если у босса то выигрыш.</t>
+  </si>
+  <si>
+    <t>Исправить диалог - Цель игры - сейчас не только расчистка!!!</t>
+  </si>
+  <si>
+    <t>Исправить диалог - перетяни оружие на оранжевую клетку для разрушения</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -448,7 +506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -463,10 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -502,24 +557,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -532,12 +569,42 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -854,18 +921,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F451F162-DA5E-CB4E-80A2-CA53019693C0}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="58.33203125" customWidth="1"/>
+    <col min="2" max="2" width="72.33203125" customWidth="1"/>
     <col min="3" max="3" width="59.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" customWidth="1"/>
+    <col min="6" max="7" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -878,159 +947,291 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>4</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>5</v>
       </c>
-      <c r="B3" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="B11" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>7</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>8</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>10</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>12</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="D22" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>6</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>7</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="8"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B22:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1052,7 +1253,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="26" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1065,13 +1266,13 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="26" t="s">
         <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="29">
         <f>128/1038</f>
         <v>0.1233140655105973</v>
       </c>
@@ -1080,12 +1281,12 @@
       <c r="C7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="29">
         <f>145/524</f>
         <v>0.27671755725190839</v>
       </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
@@ -1093,28 +1294,28 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C12" s="32">
+      <c r="C12" s="25">
         <v>43948</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="28">
         <f>94/243</f>
         <v>0.38683127572016462</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C13" s="32">
+      <c r="C13" s="25">
         <v>43949</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="28">
         <f>132/181</f>
         <v>0.72928176795580113</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C14" s="32">
+      <c r="C14" s="25">
         <v>43950</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="27">
         <f>67/5</f>
         <v>13.4</v>
       </c>
@@ -1140,66 +1341,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="25" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="25" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="25" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="25" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="25" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1224,94 +1425,94 @@
     <col min="13" max="13" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="G7" s="23" t="s">
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="G7" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="24"/>
-      <c r="I7" s="25"/>
-      <c r="L7" s="23" t="s">
+      <c r="H7" s="36"/>
+      <c r="I7" s="37"/>
+      <c r="L7" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="25"/>
+      <c r="M7" s="37"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="15"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="14"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="14"/>
     </row>
     <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.2">
-      <c r="B9" s="16"/>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="G9" s="27" t="s">
+      <c r="D9" s="17"/>
+      <c r="G9" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="28"/>
-      <c r="L9" s="31" t="s">
+      <c r="H9" s="39"/>
+      <c r="I9" s="40"/>
+      <c r="L9" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="15"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="B10" s="13"/>
-      <c r="C10" s="19">
+      <c r="B10" s="12"/>
+      <c r="C10" s="18">
         <v>3</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="G10" s="29">
+      <c r="D10" s="14"/>
+      <c r="G10" s="22">
         <v>3</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="30">
+      <c r="H10" s="13"/>
+      <c r="I10" s="23">
         <v>2</v>
       </c>
-      <c r="L10" s="16" t="s">
+      <c r="L10" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="M10" s="15"/>
+      <c r="M10" s="14"/>
     </row>
     <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="22"/>
-      <c r="L11" s="16" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="21"/>
+      <c r="L11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="M11" s="15"/>
+      <c r="M11" s="14"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L12" s="13"/>
-      <c r="M12" s="15"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L13" s="13"/>
-      <c r="M13" s="15"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L14" s="20"/>
-      <c r="M14" s="22"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="21"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">

</xml_diff>

<commit_message>
EnemyKnight fight points added.
</commit_message>
<xml_diff>
--- a/План доработок.xlsx
+++ b/План доработок.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/v_triputin/AndroidStudioProjects/CradleOfTronesGDX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8F55B3-B2B1-FF45-A76A-FA71D6D1D13D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA46E061-8D11-CD46-AEDD-E45C1CC4C9B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="4" xr2:uid="{342D1634-4B6E-1C49-B973-0F169133A098}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
   <si>
     <t>Если выделено, то нельзя отменить выделение</t>
   </si>
@@ -290,6 +290,12 @@
   </si>
   <si>
     <t>Ход -выстрел в противника (сила зависит от кол-ва собранных подряд ресурсов.</t>
+  </si>
+  <si>
+    <t>AttackTargetInfo.knightParamsForAttack.HealthPoints</t>
+  </si>
+  <si>
+    <t>Применить при атаке, т.е. Это общее число, а надо где то хранить текущее после ударов.</t>
   </si>
 </sst>
 </file>
@@ -752,8 +758,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>206714</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>11073</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -851,8 +857,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>253999</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142958</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -901,8 +907,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>113974</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -951,8 +957,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>113974</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1952,52 +1958,69 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB912C3-2481-3542-9D36-00A18230F8D5}">
-  <dimension ref="N2:O7"/>
+  <dimension ref="N2:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="15" max="15" width="46.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N2">
+    <row r="2" spans="14:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="N2" s="1">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N3">
+    <row r="3" spans="14:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="N3" s="1">
         <v>2</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N4">
+    <row r="4" spans="14:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="N4" s="1">
         <v>3</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N6">
+    <row r="5" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="N5" s="1"/>
+      <c r="O5" s="4"/>
+    </row>
+    <row r="6" spans="14:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="N6" s="1">
         <v>4</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N7">
+    <row r="7" spans="14:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="N7" s="1">
         <v>5</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="4" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="N10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="O11" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>